<commit_message>
feature: transition to multi-lang app completed adding excel file translations
</commit_message>
<xml_diff>
--- a/static/xlsx/en/Team.xlsx
+++ b/static/xlsx/en/Team.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9144"/>
+    <workbookView windowWidth="9660" windowHeight="3623"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -173,7 +173,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,19 +199,6 @@
       <color rgb="FF800080"/>
       <name val="Arial"/>
       <charset val="0"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -676,19 +663,28 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -697,127 +693,118 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -828,7 +815,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1178,7 +1165,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="3"/>

</xml_diff>